<commit_message>
Arreglada configuracion 70017048 (TIG) y subida de resultados
</commit_message>
<xml_diff>
--- a/AI_Engine/Resultados/Resultados buenos/dataFrame - 70017869.xlsx
+++ b/AI_Engine/Resultados/Resultados buenos/dataFrame - 70017869.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proyectos\Nueva carpeta\Bot-Creacion-de-Pedidos\AI_Engine\Resultados\Resultados buenos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF20296-279A-40C9-AE54-5B1E49FA00BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8FF913-9CC7-4CB5-AA64-AF42A5976251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11070" yWindow="3150" windowWidth="7905" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3720" yWindow="4155" windowWidth="7905" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>archivo</t>
   </si>
@@ -67,15 +67,9 @@
     <t>70017869</t>
   </si>
   <si>
-    <t>32.90</t>
-  </si>
-  <si>
     <t>January 10, 2023</t>
   </si>
   <si>
-    <t>R523409</t>
-  </si>
-  <si>
     <t>150.000</t>
   </si>
   <si>
@@ -133,16 +127,22 @@
     <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\TIG\t96.pdf</t>
   </si>
   <si>
-    <t>Referencia y fallo en regex con qty</t>
-  </si>
-  <si>
     <t>Que referencia es?</t>
   </si>
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>Qty</t>
+    <t>100.000</t>
+  </si>
+  <si>
+    <t>RE529419</t>
+  </si>
+  <si>
+    <t>R104589</t>
+  </si>
+  <si>
+    <t>1,000.000</t>
   </si>
 </sst>
 </file>
@@ -161,6 +161,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -511,7 +512,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,17 +560,20 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
       <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
       <c r="I2">
-        <v>-100</v>
+        <v>28.233000000000001</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -586,22 +590,22 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I3">
-        <v>66.295000000000002</v>
+        <v>91.614000000000004</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -609,28 +613,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
       <c r="I4">
-        <v>57.999000000000002</v>
+        <v>88.629000000000005</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -638,28 +642,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
       <c r="I5">
-        <v>73.037999999999997</v>
+        <v>89.540999999999997</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -667,28 +671,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I6">
-        <v>73.037999999999997</v>
+        <v>89.540999999999997</v>
       </c>
       <c r="J6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -696,25 +700,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I7">
-        <v>-100</v>
+        <v>37.264000000000003</v>
       </c>
       <c r="J7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -722,25 +729,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I8">
-        <v>-100</v>
+        <v>37.264000000000003</v>
       </c>
       <c r="J8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -748,28 +758,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" t="s">
-        <v>19</v>
-      </c>
       <c r="I9">
-        <v>57.999000000000002</v>
+        <v>88.629000000000005</v>
       </c>
       <c r="J9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -777,34 +787,34 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
       <c r="I10">
-        <v>73.037999999999997</v>
+        <v>89.540999999999997</v>
       </c>
       <c r="J10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12">
         <f>AVERAGEIF(I2:I10,"&lt;&gt;-100")</f>
-        <v>66.901166666666668</v>
+        <v>71.13955555555556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios coordenadas qty en TIG
</commit_message>
<xml_diff>
--- a/AI_Engine/Resultados/Resultados buenos/dataFrame - 70017869.xlsx
+++ b/AI_Engine/Resultados/Resultados buenos/dataFrame - 70017869.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deere-my.sharepoint.com/personal/gonzalezdiazsergio_johndeere_com/Documents/Desktop/Proyectos/Bot-Creacion-de-Pedidos/AI_Engine/Resultados/Resultados buenos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{0D8FF913-9CC7-4CB5-AA64-AF42A5976251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFAA0CA5-28C6-48BC-B67C-C51DFD9E4E28}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{0D8FF913-9CC7-4CB5-AA64-AF42A5976251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7998C3D-8188-40FA-9FC4-8221868147ED}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="-1020" windowWidth="13950" windowHeight="11550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="0" windowWidth="20925" windowHeight="16995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,13 +133,13 @@
     <t>100.000</t>
   </si>
   <si>
-    <t>RE529419</t>
-  </si>
-  <si>
     <t>R104589</t>
   </si>
   <si>
     <t>1,000.000</t>
+  </si>
+  <si>
+    <t>R523409</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="I2" sqref="I2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
@@ -587,7 +587,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -596,7 +596,7 @@
         <v>11</v>
       </c>
       <c r="I3">
-        <v>90.263000000000005</v>
+        <v>89.906999999999996</v>
       </c>
       <c r="J3" t="s">
         <v>31</v>
@@ -706,7 +706,7 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
@@ -735,7 +735,7 @@
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
         <v>28</v>
@@ -808,7 +808,7 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I12">
         <f>AVERAGEIF(I2:I10,"&lt;&gt;-100")</f>
-        <v>90.592111111111123</v>
+        <v>90.552555555555557</v>
       </c>
     </row>
   </sheetData>

</xml_diff>